<commit_message>
Last updated at 12:07 AM
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>User_Role</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>448924A</t>
+  </si>
+  <si>
+    <t>5FA3C2312892FD51F30690CB47131C4C</t>
+  </si>
+  <si>
+    <t>4482716A</t>
   </si>
 </sst>
 </file>
@@ -604,7 +610,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>
@@ -772,7 +778,7 @@
         <v>38</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Change in chrome driver
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
   <si>
     <t>User_Role</t>
   </si>
@@ -220,6 +220,132 @@
   </si>
   <si>
     <t>4482716A</t>
+  </si>
+  <si>
+    <t>21CD404E2CF61617089F7772AC0F14E7</t>
+  </si>
+  <si>
+    <t>Image_Add</t>
+  </si>
+  <si>
+    <t>10500</t>
+  </si>
+  <si>
+    <t>1D6D71E7EDB897B0DE87685696AAB905</t>
+  </si>
+  <si>
+    <t>9DB7431A91BA0657B88111C7586B67EE</t>
+  </si>
+  <si>
+    <t>33D70E88F03087A7D38D1BD3F178FE8D</t>
+  </si>
+  <si>
+    <t>1527F847E65DAE8BF2FFD695CFCB15BC</t>
+  </si>
+  <si>
+    <t>3A94A50A324859CF012210B5A0DCC35A</t>
+  </si>
+  <si>
+    <t>C6545E4A44157B9361C62B89DCE6183F</t>
+  </si>
+  <si>
+    <t>54E031405B66B3DA824DF48CABBF600E</t>
+  </si>
+  <si>
+    <t>E7D0D951EFAF7BD9EE8C9C42E6068FD1</t>
+  </si>
+  <si>
+    <t>CB61A006A040E8E594BB17BE40CBE344</t>
+  </si>
+  <si>
+    <t>C04DB5BD5FF792F4222E66218182EC7F</t>
+  </si>
+  <si>
+    <t>15FAE3AB82C844F74BE59155B1F56264</t>
+  </si>
+  <si>
+    <t>277B5B6F330B47D66B301795D202B069</t>
+  </si>
+  <si>
+    <t>071F42BD0259AC76987B34130F8CC164</t>
+  </si>
+  <si>
+    <t>58D7A2408E5B9C03B9AC916932FBB8E1</t>
+  </si>
+  <si>
+    <t>298FA4EB6240273A4625010C7BA7715A</t>
+  </si>
+  <si>
+    <t>DCB4B10F7D04DB64AB9F03DB46604993</t>
+  </si>
+  <si>
+    <t>PersonalDetails</t>
+  </si>
+  <si>
+    <t>10600</t>
+  </si>
+  <si>
+    <t>2CB5F0CE8494A72AAD9C17DAF760CFEB</t>
+  </si>
+  <si>
+    <t>4A0AC1F28A22CF9DB1689BE18F055B9D</t>
+  </si>
+  <si>
+    <t>D2871CC68E2F80BFF73A01A8D4F9ADD7</t>
+  </si>
+  <si>
+    <t>D28C8DF361EFA2D1E3279C62AF76C02A</t>
+  </si>
+  <si>
+    <t>D27CD39967D3941E2007CD1D97134F93</t>
+  </si>
+  <si>
+    <t>78B4E520665578A91E5A293AA5EDFE56</t>
+  </si>
+  <si>
+    <t>9BE899E9A625DEB2CA045F6A1B40D8E4</t>
+  </si>
+  <si>
+    <t>2E8BB6093357E2A3399192B724D85A84</t>
+  </si>
+  <si>
+    <t>623312DDD2D46FCC737BC6588A8D607B</t>
+  </si>
+  <si>
+    <t>5F55AD6B38C8487124E6A4EE1E6141E5</t>
+  </si>
+  <si>
+    <t>6522549098833C6CE84D428E9D938F2B</t>
+  </si>
+  <si>
+    <t>1BB85177D85A4CC3FC8DF4DB6F0FD0BA</t>
+  </si>
+  <si>
+    <t>0D46C29E4B13DFB317EA2DE427C0F07E</t>
+  </si>
+  <si>
+    <t>681159B99151C4560208968DF9CA6B85</t>
+  </si>
+  <si>
+    <t>21A2C0D654A2BDD635CA614AAA069F56</t>
+  </si>
+  <si>
+    <t>A3CD14971698933F7778902DCD29C6D1</t>
+  </si>
+  <si>
+    <t>75542AF361A5DF9446F69D05E6D7C6F7</t>
+  </si>
+  <si>
+    <t>51C4B9CBC024E784BCE05B3119D0BA31</t>
+  </si>
+  <si>
+    <t>712745A</t>
+  </si>
+  <si>
+    <t>C740395689588328E5DA6BCCD7E88F35</t>
+  </si>
+  <si>
+    <t>1342182A</t>
   </si>
 </sst>
 </file>
@@ -610,7 +736,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>
@@ -778,15 +904,15 @@
         <v>38</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>65</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>60</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addee new version chromedriver
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856" activeTab="2"/>
+    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
     <sheet name="Personal" sheetId="2" r:id="rId2"/>
     <sheet name="Jira" sheetId="3" r:id="rId3"/>
+    <sheet name="Available Busses" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="108">
   <si>
     <t>User_Role</t>
   </si>
@@ -126,9 +127,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>2341381A</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -138,214 +136,214 @@
     <t>Key</t>
   </si>
   <si>
-    <t>AccessRecords</t>
-  </si>
-  <si>
-    <t>4E6067F8E39D2786256F2BED79A03D4D</t>
-  </si>
-  <si>
-    <t>10300</t>
-  </si>
-  <si>
-    <t>C501B37C673E3148AE79546E55127AF6</t>
-  </si>
-  <si>
-    <t>7A1518C846D2C5DA248FCE8585242F39</t>
-  </si>
-  <si>
-    <t>D4F509033048B97B65FF845B2C906141</t>
-  </si>
-  <si>
-    <t>C422503A5AEF903B0AB25ED52F8ECF3D</t>
-  </si>
-  <si>
-    <t>147BE00AD5E6A19CC045D7B239D68AA1</t>
-  </si>
-  <si>
-    <t>B825142C546D0564A7FE05C2C1F2A33D</t>
-  </si>
-  <si>
-    <t>18EBE48759900126339A7D7D268C5905</t>
-  </si>
-  <si>
-    <t>1615AF9DC9C9FB971534BAB9D896635E</t>
-  </si>
-  <si>
-    <t>6FBEF2C5C58276ACDE4C9F4404DFA47A</t>
-  </si>
-  <si>
-    <t>1A1F98487E9AA28BDCD85998B1D99314</t>
-  </si>
-  <si>
-    <t>260FCB84D39009DC294B72D94AF535B4</t>
-  </si>
-  <si>
-    <t>4038738A</t>
-  </si>
-  <si>
-    <t>542CDC2421B5815E5C644D3C15F7C4CD</t>
-  </si>
-  <si>
-    <t>8535857A</t>
-  </si>
-  <si>
-    <t>33C22F19FC50FF5B51D04030974F2284</t>
-  </si>
-  <si>
-    <t>3264250A</t>
-  </si>
-  <si>
-    <t>E285D47C5FA737974E452BC0A51E736F</t>
-  </si>
-  <si>
-    <t>Admin_SystemUsername</t>
-  </si>
-  <si>
-    <t>10400</t>
-  </si>
-  <si>
-    <t>A992A297C8F4AC6FBA707DCBF68040C1</t>
-  </si>
-  <si>
-    <t>2323489A</t>
-  </si>
-  <si>
-    <t>0C6E5E6E11D4DE9764C9A5F1C9073D27</t>
-  </si>
-  <si>
-    <t>448924A</t>
-  </si>
-  <si>
-    <t>5FA3C2312892FD51F30690CB47131C4C</t>
-  </si>
-  <si>
-    <t>4482716A</t>
-  </si>
-  <si>
-    <t>21CD404E2CF61617089F7772AC0F14E7</t>
-  </si>
-  <si>
-    <t>Image_Add</t>
-  </si>
-  <si>
-    <t>10500</t>
-  </si>
-  <si>
-    <t>1D6D71E7EDB897B0DE87685696AAB905</t>
-  </si>
-  <si>
-    <t>9DB7431A91BA0657B88111C7586B67EE</t>
-  </si>
-  <si>
-    <t>33D70E88F03087A7D38D1BD3F178FE8D</t>
-  </si>
-  <si>
-    <t>1527F847E65DAE8BF2FFD695CFCB15BC</t>
-  </si>
-  <si>
-    <t>3A94A50A324859CF012210B5A0DCC35A</t>
-  </si>
-  <si>
-    <t>C6545E4A44157B9361C62B89DCE6183F</t>
-  </si>
-  <si>
-    <t>54E031405B66B3DA824DF48CABBF600E</t>
-  </si>
-  <si>
-    <t>E7D0D951EFAF7BD9EE8C9C42E6068FD1</t>
-  </si>
-  <si>
-    <t>CB61A006A040E8E594BB17BE40CBE344</t>
-  </si>
-  <si>
-    <t>C04DB5BD5FF792F4222E66218182EC7F</t>
-  </si>
-  <si>
-    <t>15FAE3AB82C844F74BE59155B1F56264</t>
-  </si>
-  <si>
-    <t>277B5B6F330B47D66B301795D202B069</t>
-  </si>
-  <si>
-    <t>071F42BD0259AC76987B34130F8CC164</t>
-  </si>
-  <si>
-    <t>58D7A2408E5B9C03B9AC916932FBB8E1</t>
-  </si>
-  <si>
-    <t>298FA4EB6240273A4625010C7BA7715A</t>
-  </si>
-  <si>
-    <t>DCB4B10F7D04DB64AB9F03DB46604993</t>
-  </si>
-  <si>
-    <t>PersonalDetails</t>
-  </si>
-  <si>
-    <t>10600</t>
-  </si>
-  <si>
-    <t>2CB5F0CE8494A72AAD9C17DAF760CFEB</t>
-  </si>
-  <si>
-    <t>4A0AC1F28A22CF9DB1689BE18F055B9D</t>
-  </si>
-  <si>
-    <t>D2871CC68E2F80BFF73A01A8D4F9ADD7</t>
-  </si>
-  <si>
-    <t>D28C8DF361EFA2D1E3279C62AF76C02A</t>
-  </si>
-  <si>
-    <t>D27CD39967D3941E2007CD1D97134F93</t>
-  </si>
-  <si>
-    <t>78B4E520665578A91E5A293AA5EDFE56</t>
-  </si>
-  <si>
-    <t>9BE899E9A625DEB2CA045F6A1B40D8E4</t>
-  </si>
-  <si>
-    <t>2E8BB6093357E2A3399192B724D85A84</t>
-  </si>
-  <si>
-    <t>623312DDD2D46FCC737BC6588A8D607B</t>
-  </si>
-  <si>
-    <t>5F55AD6B38C8487124E6A4EE1E6141E5</t>
-  </si>
-  <si>
-    <t>6522549098833C6CE84D428E9D938F2B</t>
-  </si>
-  <si>
-    <t>1BB85177D85A4CC3FC8DF4DB6F0FD0BA</t>
-  </si>
-  <si>
-    <t>0D46C29E4B13DFB317EA2DE427C0F07E</t>
-  </si>
-  <si>
-    <t>681159B99151C4560208968DF9CA6B85</t>
-  </si>
-  <si>
-    <t>21A2C0D654A2BDD635CA614AAA069F56</t>
-  </si>
-  <si>
-    <t>A3CD14971698933F7778902DCD29C6D1</t>
-  </si>
-  <si>
-    <t>75542AF361A5DF9446F69D05E6D7C6F7</t>
-  </si>
-  <si>
-    <t>51C4B9CBC024E784BCE05B3119D0BA31</t>
-  </si>
-  <si>
-    <t>712745A</t>
-  </si>
-  <si>
-    <t>C740395689588328E5DA6BCCD7E88F35</t>
-  </si>
-  <si>
-    <t>1342182A</t>
+    <t>6750410A</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>Busses Name</t>
+  </si>
+  <si>
+    <t>Departure time</t>
+  </si>
+  <si>
+    <t>Old Amount</t>
+  </si>
+  <si>
+    <t>New Amount</t>
+  </si>
+  <si>
+    <t>557630E607A00849AA32E74CFD171531</t>
+  </si>
+  <si>
+    <t>A008E31A600FABC2F659D0740BC0CCC1</t>
+  </si>
+  <si>
+    <t>C9853342596B17457644025C3E7ECA48</t>
+  </si>
+  <si>
+    <t>648C1FB615690CD7DF9E5AF52208C631</t>
+  </si>
+  <si>
+    <t>7A894449E60C1484052B9E063CB06131</t>
+  </si>
+  <si>
+    <t>ADB68E4B3DC5EBD05793238AF2D4F7E0</t>
+  </si>
+  <si>
+    <t>8BE0FC4953B9FBE94CD252DF65B0C27D</t>
+  </si>
+  <si>
+    <t>3A66000E7F14793DB464E9CF8893A7CD</t>
+  </si>
+  <si>
+    <t>79D5A9EE4F8D2D7FE474F234619E8DB9</t>
+  </si>
+  <si>
+    <t>Sabari Travels</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>850</t>
+  </si>
+  <si>
+    <t>765</t>
+  </si>
+  <si>
+    <t>JB Connect</t>
+  </si>
+  <si>
+    <t>21:10</t>
+  </si>
+  <si>
+    <t>1340</t>
+  </si>
+  <si>
+    <t>SPS Travels</t>
+  </si>
+  <si>
+    <t>20:40</t>
+  </si>
+  <si>
+    <t>790</t>
+  </si>
+  <si>
+    <t>740</t>
+  </si>
+  <si>
+    <t>AdSHRI AANJANEYA TRAVELS</t>
+  </si>
+  <si>
+    <t>21:15</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>Chakra Travels</t>
+  </si>
+  <si>
+    <t>21:45</t>
+  </si>
+  <si>
+    <t>840</t>
+  </si>
+  <si>
+    <t>SST LIMOLINER</t>
+  </si>
+  <si>
+    <t>899</t>
+  </si>
+  <si>
+    <t>849</t>
+  </si>
+  <si>
+    <t>20:45</t>
+  </si>
+  <si>
+    <t>Krish Bus</t>
+  </si>
+  <si>
+    <t>20:30</t>
+  </si>
+  <si>
+    <t>21:40</t>
+  </si>
+  <si>
+    <t>SNB Travels</t>
+  </si>
+  <si>
+    <t>23:00</t>
+  </si>
+  <si>
+    <t>IntrCity SmartBus</t>
+  </si>
+  <si>
+    <t>1051</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>22:10</t>
+  </si>
+  <si>
+    <t>A1 Travels</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>PSS Transport</t>
+  </si>
+  <si>
+    <t>22:00</t>
+  </si>
+  <si>
+    <t>Krish Travels</t>
+  </si>
+  <si>
+    <t>20:15</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>LION Travels</t>
+  </si>
+  <si>
+    <t>900</t>
+  </si>
+  <si>
+    <t>Tranz king travels</t>
+  </si>
+  <si>
+    <t>22:15</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Samantha'S Travels</t>
+  </si>
+  <si>
+    <t>18:50</t>
+  </si>
+  <si>
+    <t>950</t>
+  </si>
+  <si>
+    <t>875</t>
+  </si>
+  <si>
+    <t>YBM Travels(BLM)</t>
+  </si>
+  <si>
+    <t>960</t>
+  </si>
+  <si>
+    <t>910</t>
+  </si>
+  <si>
+    <t>ARS TRAVELS</t>
+  </si>
+  <si>
+    <t>21:30</t>
+  </si>
+  <si>
+    <t>BSP Bus</t>
+  </si>
+  <si>
+    <t>4E01BFB9ECC60107D17AA08AED3C3A3F</t>
+  </si>
+  <si>
+    <t>3869E2724283957C0CA35A98BA69CA28</t>
+  </si>
+  <si>
+    <t>6042875A</t>
   </si>
 </sst>
 </file>
@@ -736,7 +734,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>
@@ -881,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -893,26 +891,317 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s" s="0">
         <v>36</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="B3" s="0"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.6640625"/>
+    <col min="2" max="2" customWidth="true" width="18.21875"/>
+    <col min="3" max="3" customWidth="true" width="12.5546875"/>
+    <col min="4" max="4" customWidth="true" width="12.33203125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>87</v>
+      <c r="D18" t="s" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to code to run all test without fail expect for leave test case
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="151">
   <si>
     <t>User_Role</t>
   </si>
@@ -344,6 +344,135 @@
   </si>
   <si>
     <t>6042875A</t>
+  </si>
+  <si>
+    <t>BB323B47F46E5CD42F3497455DBFD9E3</t>
+  </si>
+  <si>
+    <t>6453366A</t>
+  </si>
+  <si>
+    <t>FE136E670451A46D7D4DD0AA0585FAC2</t>
+  </si>
+  <si>
+    <t>6954595A</t>
+  </si>
+  <si>
+    <t>A4D33CB5B00C6D5ED0C35CAD03B1ACB9</t>
+  </si>
+  <si>
+    <t>Recruitment_HiredList</t>
+  </si>
+  <si>
+    <t>Recruitment_RejectionList1</t>
+  </si>
+  <si>
+    <t>FE95D2FD09506C0C6A430405CC965BF9</t>
+  </si>
+  <si>
+    <t>57F9A8A125A1E93AD758458F9CF33437</t>
+  </si>
+  <si>
+    <t>C368C7E10B90663D5CAA8DCF33B48C03</t>
+  </si>
+  <si>
+    <t>4299C73D6D63E36590B0A3DEDF80495E</t>
+  </si>
+  <si>
+    <t>Leave_Accept</t>
+  </si>
+  <si>
+    <t>84614D0142BEBB135BBAB5C8DF574CBA</t>
+  </si>
+  <si>
+    <t>715D3F3C0AE52C199FA9BFFDA639690C</t>
+  </si>
+  <si>
+    <t>079E10170773E7C5CF84DB83E5818772</t>
+  </si>
+  <si>
+    <t>PersonalDetails</t>
+  </si>
+  <si>
+    <t>47226E02BF491C2871895A11DC253190</t>
+  </si>
+  <si>
+    <t>7D41F787680F2BA53D1493C96DB27EA5</t>
+  </si>
+  <si>
+    <t>6BEB6266E2BD431EA62FAB4ECE15BB18</t>
+  </si>
+  <si>
+    <t>23F10278A54C130A85438DDB17C74920</t>
+  </si>
+  <si>
+    <t>884FC19FFE846E17D560261FE56BAB12</t>
+  </si>
+  <si>
+    <t>F9222770CFF8BA12FA042592224A5DCE</t>
+  </si>
+  <si>
+    <t>704816DDC7DAD31D1ED859A56254F7CC</t>
+  </si>
+  <si>
+    <t>6C8A46F036765EDC64182BC5C03140E2</t>
+  </si>
+  <si>
+    <t>3D572D2C7CC117473D9213970A53872D</t>
+  </si>
+  <si>
+    <t>4415F51FD9AFA87FFE6411DE9C1DF626</t>
+  </si>
+  <si>
+    <t>PIM_AddEmployee</t>
+  </si>
+  <si>
+    <t>470E9187B8B7CD2069F68BF075529197</t>
+  </si>
+  <si>
+    <t>FBAAD7B3B94F6A4A89199466E078038D</t>
+  </si>
+  <si>
+    <t>0BF451527A03FB96BBDE6839B2C9C290</t>
+  </si>
+  <si>
+    <t>7284198A</t>
+  </si>
+  <si>
+    <t>90156D586D70B66DA8FA67CAC75FB374</t>
+  </si>
+  <si>
+    <t>1526161A</t>
+  </si>
+  <si>
+    <t>F0D37F9591A97CC8DEF388D13BB9EDFF</t>
+  </si>
+  <si>
+    <t>7064986A</t>
+  </si>
+  <si>
+    <t>FB66223C05D3646126187994AD064B5F</t>
+  </si>
+  <si>
+    <t>210D5EDFB1EF3DD9091193C018CE62D9</t>
+  </si>
+  <si>
+    <t>EEAE04DD267BF3908C0DCC71A668D1BF</t>
+  </si>
+  <si>
+    <t>1A06CCD99FE1FA001AF8A201CB4B1330</t>
+  </si>
+  <si>
+    <t>EB2E0A01A90A98D0C627E2E06ABD23B2</t>
+  </si>
+  <si>
+    <t>3E6052428FA505F328C3BF7D80F73036</t>
+  </si>
+  <si>
+    <t>2098D84319E1DC7FC1B341BAEF3278E0</t>
+  </si>
+  <si>
+    <t>0E8CAC993B05BCDF8711C30890361286</t>
   </si>
 </sst>
 </file>
@@ -734,7 +863,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>
@@ -877,7 +1006,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -902,14 +1031,20 @@
         <v>37</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>106</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="B3" s="0"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="B4" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes in pom file for plugin
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="153">
   <si>
     <t>User_Role</t>
   </si>
@@ -473,6 +473,12 @@
   </si>
   <si>
     <t>0E8CAC993B05BCDF8711C30890361286</t>
+  </si>
+  <si>
+    <t>84BD033C7474FC853CA2D183F92C5BD8</t>
+  </si>
+  <si>
+    <t>0510BF5830A993F63C406F342D7B53F7</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1037,7 @@
         <v>37</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Latest code change for github run
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="125">
   <si>
     <t>User_Role</t>
   </si>
@@ -344,6 +344,57 @@
   </si>
   <si>
     <t>6042875A</t>
+  </si>
+  <si>
+    <t>BAA6D0641A01A8F8C01FEADB0B35542A</t>
+  </si>
+  <si>
+    <t>C629ABE4A0D2A86847F28FFEEECD7128</t>
+  </si>
+  <si>
+    <t>4FE69F7C43C1823C068DEBCDA9E272D6</t>
+  </si>
+  <si>
+    <t>Leave_Accept</t>
+  </si>
+  <si>
+    <t>Recruitment_HiredList</t>
+  </si>
+  <si>
+    <t>Recruitment_RejectionList1</t>
+  </si>
+  <si>
+    <t>PersonalDetails</t>
+  </si>
+  <si>
+    <t>311A0B7F309C08F0DA83165527C90454</t>
+  </si>
+  <si>
+    <t>5652C61FF0A4A5724C23BE971B2A3958</t>
+  </si>
+  <si>
+    <t>7940051A</t>
+  </si>
+  <si>
+    <t>FA364E3703878AAF51D9BC55ECC85704</t>
+  </si>
+  <si>
+    <t>1260060A</t>
+  </si>
+  <si>
+    <t>9980824A</t>
+  </si>
+  <si>
+    <t>B858ABB95D2192E65C93CEA119C54A20</t>
+  </si>
+  <si>
+    <t>831407A</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>7598587A</t>
   </si>
 </sst>
 </file>
@@ -734,7 +785,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>
@@ -877,7 +928,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -902,14 +953,34 @@
         <v>37</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>106</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="B3" s="0"/>
+        <v>114</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="B4" s="0"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="B5" s="0"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="B6" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
All test to run changes in testng
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="128">
   <si>
     <t>User_Role</t>
   </si>
@@ -395,6 +395,15 @@
   </si>
   <si>
     <t>7598587A</t>
+  </si>
+  <si>
+    <t>Recruitment_Rejected1</t>
+  </si>
+  <si>
+    <t>1036771A</t>
+  </si>
+  <si>
+    <t>8448782A</t>
   </si>
 </sst>
 </file>
@@ -785,7 +794,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>
@@ -958,7 +967,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>123</v>
@@ -966,9 +975,11 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>112</v>
-      </c>
-      <c r="B4" s="0"/>
+        <v>125</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>123</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">

</xml_diff>

<commit_message>
Changed local db as docker db
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="130">
   <si>
     <t>User_Role</t>
   </si>
@@ -404,6 +404,12 @@
   </si>
   <si>
     <t>8448782A</t>
+  </si>
+  <si>
+    <t>4044786A</t>
+  </si>
+  <si>
+    <t>1495934A</t>
   </si>
 </sst>
 </file>
@@ -794,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>
@@ -967,7 +973,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>123</v>

</xml_diff>

<commit_message>
Some code changes for running in github
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856" activeTab="3"/>
+    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
   <si>
     <t>User_Role</t>
   </si>
@@ -136,12 +136,6 @@
     <t>Key</t>
   </si>
   <si>
-    <t>6750410A</t>
-  </si>
-  <si>
-    <t>run</t>
-  </si>
-  <si>
     <t>Busses Name</t>
   </si>
   <si>
@@ -154,36 +148,6 @@
     <t>New Amount</t>
   </si>
   <si>
-    <t>557630E607A00849AA32E74CFD171531</t>
-  </si>
-  <si>
-    <t>A008E31A600FABC2F659D0740BC0CCC1</t>
-  </si>
-  <si>
-    <t>C9853342596B17457644025C3E7ECA48</t>
-  </si>
-  <si>
-    <t>648C1FB615690CD7DF9E5AF52208C631</t>
-  </si>
-  <si>
-    <t>7A894449E60C1484052B9E063CB06131</t>
-  </si>
-  <si>
-    <t>ADB68E4B3DC5EBD05793238AF2D4F7E0</t>
-  </si>
-  <si>
-    <t>8BE0FC4953B9FBE94CD252DF65B0C27D</t>
-  </si>
-  <si>
-    <t>3A66000E7F14793DB464E9CF8893A7CD</t>
-  </si>
-  <si>
-    <t>79D5A9EE4F8D2D7FE474F234619E8DB9</t>
-  </si>
-  <si>
-    <t>Sabari Travels</t>
-  </si>
-  <si>
     <t>21:00</t>
   </si>
   <si>
@@ -193,18 +157,12 @@
     <t>765</t>
   </si>
   <si>
-    <t>JB Connect</t>
-  </si>
-  <si>
     <t>21:10</t>
   </si>
   <si>
     <t>1340</t>
   </si>
   <si>
-    <t>SPS Travels</t>
-  </si>
-  <si>
     <t>20:40</t>
   </si>
   <si>
@@ -214,27 +172,18 @@
     <t>740</t>
   </si>
   <si>
-    <t>AdSHRI AANJANEYA TRAVELS</t>
-  </si>
-  <si>
     <t>21:15</t>
   </si>
   <si>
     <t>800</t>
   </si>
   <si>
-    <t>Chakra Travels</t>
-  </si>
-  <si>
     <t>21:45</t>
   </si>
   <si>
     <t>840</t>
   </si>
   <si>
-    <t>SST LIMOLINER</t>
-  </si>
-  <si>
     <t>899</t>
   </si>
   <si>
@@ -244,24 +193,15 @@
     <t>20:45</t>
   </si>
   <si>
-    <t>Krish Bus</t>
-  </si>
-  <si>
     <t>20:30</t>
   </si>
   <si>
     <t>21:40</t>
   </si>
   <si>
-    <t>SNB Travels</t>
-  </si>
-  <si>
     <t>23:00</t>
   </si>
   <si>
-    <t>IntrCity SmartBus</t>
-  </si>
-  <si>
     <t>1051</t>
   </si>
   <si>
@@ -271,45 +211,27 @@
     <t>22:10</t>
   </si>
   <si>
-    <t>A1 Travels</t>
-  </si>
-  <si>
     <t>700</t>
   </si>
   <si>
-    <t>PSS Transport</t>
-  </si>
-  <si>
     <t>22:00</t>
   </si>
   <si>
-    <t>Krish Travels</t>
-  </si>
-  <si>
     <t>20:15</t>
   </si>
   <si>
     <t>500</t>
   </si>
   <si>
-    <t>LION Travels</t>
-  </si>
-  <si>
     <t>900</t>
   </si>
   <si>
-    <t>Tranz king travels</t>
-  </si>
-  <si>
     <t>22:15</t>
   </si>
   <si>
     <t>1000</t>
   </si>
   <si>
-    <t>Samantha'S Travels</t>
-  </si>
-  <si>
     <t>18:50</t>
   </si>
   <si>
@@ -319,97 +241,34 @@
     <t>875</t>
   </si>
   <si>
-    <t>YBM Travels(BLM)</t>
-  </si>
-  <si>
     <t>960</t>
   </si>
   <si>
     <t>910</t>
   </si>
   <si>
-    <t>ARS TRAVELS</t>
-  </si>
-  <si>
     <t>21:30</t>
   </si>
   <si>
-    <t>BSP Bus</t>
-  </si>
-  <si>
-    <t>4E01BFB9ECC60107D17AA08AED3C3A3F</t>
-  </si>
-  <si>
-    <t>3869E2724283957C0CA35A98BA69CA28</t>
-  </si>
-  <si>
-    <t>6042875A</t>
-  </si>
-  <si>
-    <t>BAA6D0641A01A8F8C01FEADB0B35542A</t>
-  </si>
-  <si>
-    <t>C629ABE4A0D2A86847F28FFEEECD7128</t>
-  </si>
-  <si>
-    <t>4FE69F7C43C1823C068DEBCDA9E272D6</t>
-  </si>
-  <si>
-    <t>Leave_Accept</t>
-  </si>
-  <si>
-    <t>Recruitment_HiredList</t>
-  </si>
-  <si>
     <t>Recruitment_RejectionList1</t>
   </si>
   <si>
     <t>PersonalDetails</t>
   </si>
   <si>
-    <t>311A0B7F309C08F0DA83165527C90454</t>
-  </si>
-  <si>
-    <t>5652C61FF0A4A5724C23BE971B2A3958</t>
-  </si>
-  <si>
-    <t>7940051A</t>
-  </si>
-  <si>
-    <t>FA364E3703878AAF51D9BC55ECC85704</t>
-  </si>
-  <si>
-    <t>1260060A</t>
-  </si>
-  <si>
-    <t>9980824A</t>
-  </si>
-  <si>
-    <t>B858ABB95D2192E65C93CEA119C54A20</t>
-  </si>
-  <si>
-    <t>831407A</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>7598587A</t>
-  </si>
-  <si>
     <t>Recruitment_Rejected1</t>
   </si>
   <si>
-    <t>1036771A</t>
-  </si>
-  <si>
-    <t>8448782A</t>
-  </si>
-  <si>
-    <t>4044786A</t>
-  </si>
-  <si>
-    <t>1495934A</t>
+    <t>5486487A</t>
+  </si>
+  <si>
+    <t>59619A</t>
+  </si>
+  <si>
+    <t>4630042A</t>
   </si>
 </sst>
 </file>
@@ -755,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,7 +659,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>
@@ -968,36 +827,34 @@
         <v>37</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="B5" s="0"/>
-    </row>
-    <row r="6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>114</v>
-      </c>
-      <c r="B6" s="0"/>
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1008,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1022,274 +879,274 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="D1" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="C1" t="s" s="0">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="C2" t="s" s="0">
         <v>43</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="s" s="0">
+      <c r="D2" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D7" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="D2" t="s" s="0">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s" s="0">
         <v>56</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="s" s="0">
+      <c r="C8" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D10" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s" s="0">
         <v>59</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="s" s="0">
+      <c r="D12" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="C4" t="s" s="0">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="C14" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s" s="0">
         <v>63</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" t="s" s="0">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="D19" t="s" s="0">
         <v>66</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" t="s" s="0">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D21" t="s" s="0">
         <v>69</v>
       </c>
     </row>
-    <row r="7">
-      <c r="B7" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="C7" t="s" s="0">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D22" t="s" s="0">
         <v>72</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" t="s" s="0">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="0">
+      <c r="D24" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="D10" t="s" s="0">
+      <c r="C25" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s" s="0">
         <v>59</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="D14" t="s" s="0">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s" s="0">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="D18" t="s" s="0">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="D19" t="s" s="0">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="s" s="0">
+      <c r="C28" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="D28" t="s" s="0">
         <v>61</v>
-      </c>
-      <c r="D20" t="s" s="0">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="D21" t="s" s="0">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="s" s="0">
-        <v>96</v>
-      </c>
-      <c r="C22" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="D22" t="s" s="0">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="D23" t="s" s="0">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="C24" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="D24" t="s" s="0">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="s" s="0">
-        <v>103</v>
-      </c>
-      <c r="C25" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="D25" t="s" s="0">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="s" s="0">
-        <v>103</v>
-      </c>
-      <c r="D26" t="s" s="0">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="C27" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="D27" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="C28" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="D28" t="s" s="0">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added linux chromedriver for running
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="84">
   <si>
     <t>User_Role</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>4630042A</t>
+  </si>
+  <si>
+    <t>5080711A</t>
   </si>
 </sst>
 </file>
@@ -659,7 +662,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>

</xml_diff>

<commit_message>
Code changes for git run
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
   <si>
     <t>User_Role</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>5080711A</t>
+  </si>
+  <si>
+    <t>7904253A</t>
   </si>
 </sst>
 </file>
@@ -662,7 +665,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>

</xml_diff>

<commit_message>
Code change for all test work
</commit_message>
<xml_diff>
--- a/src/main/java/Repository/OrangeHRM_Excel.xlsx
+++ b/src/main/java/Repository/OrangeHRM_Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
   <si>
     <t>User_Role</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>7904253A</t>
+  </si>
+  <si>
+    <t>299196A</t>
   </si>
 </sst>
 </file>
@@ -665,7 +668,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>8</v>
@@ -836,7 +839,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" t="s" s="0">
         <v>76</v>
       </c>

</xml_diff>